<commit_message>
retirada de dados sensiveis e pastas sem uso
</commit_message>
<xml_diff>
--- a/recebidos.xlsx
+++ b/recebidos.xlsx
@@ -1,20 +1,25 @@
 
 <file path=xl/workbook.xml><?xml version="1.0" encoding="utf-8"?>
-<workbook xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships">
-  <fileVersion appName="xl" lastEdited="4" lowestEdited="4" rupBuild="4505"/>
+<workbook xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x15="http://schemas.microsoft.com/office/spreadsheetml/2010/11/main" mc:Ignorable="x15">
+  <fileVersion appName="xl" lastEdited="6" lowestEdited="4" rupBuild="14420"/>
   <workbookPr defaultThemeVersion="124226"/>
+  <mc:AlternateContent xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006">
+    <mc:Choice Requires="x15">
+      <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="C:\Users\DOCUMENTOS\Desktop\Ia orçamentos\"/>
+    </mc:Choice>
+  </mc:AlternateContent>
   <bookViews>
     <workbookView xWindow="240" yWindow="15" windowWidth="16095" windowHeight="9660"/>
   </bookViews>
   <sheets>
     <sheet name="Sheet1" sheetId="1" r:id="rId1"/>
   </sheets>
-  <calcPr calcId="124519" fullCalcOnLoad="1"/>
+  <calcPr calcId="124519"/>
 </workbook>
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="28" uniqueCount="17">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="7" uniqueCount="7">
   <si>
     <t>Nome</t>
   </si>
@@ -35,43 +40,13 @@
   </si>
   <si>
     <t>Foto</t>
-  </si>
-  <si>
-    <t>Eduardo Jose Martins</t>
-  </si>
-  <si>
-    <t>(44) 988449988</t>
-  </si>
-  <si>
-    <t>(53) 981034248</t>
-  </si>
-  <si>
-    <t>48999371726</t>
-  </si>
-  <si>
-    <t>eduardomartins@refera.com.br</t>
-  </si>
-  <si>
-    <t>Rua Expedicionário Iracy Luchina, 1212</t>
-  </si>
-  <si>
-    <t>Ibagy</t>
-  </si>
-  <si>
-    <t>residencial</t>
-  </si>
-  <si>
-    <t>comercial</t>
-  </si>
-  <si>
-    <t>Screenshot_223.png</t>
   </si>
 </sst>
 </file>
 
 <file path=xl/styles.xml><?xml version="1.0" encoding="utf-8"?>
-<styleSheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main">
-  <fonts count="2">
+<styleSheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:x16r2="http://schemas.microsoft.com/office/spreadsheetml/2015/02/main" mc:Ignorable="x14ac x16r2">
+  <fonts count="2" x14ac:knownFonts="1">
     <font>
       <sz val="11"/>
       <color theme="1"/>
@@ -134,11 +109,19 @@
   </cellStyles>
   <dxfs count="0"/>
   <tableStyles count="0" defaultTableStyle="TableStyleMedium9" defaultPivotStyle="PivotStyleLight16"/>
+  <extLst>
+    <ext xmlns:x14="http://schemas.microsoft.com/office/spreadsheetml/2009/9/main" uri="{EB79DEF2-80B8-43e5-95BD-54CBDDF9020C}">
+      <x14:slicerStyles defaultSlicerStyle="SlicerStyleLight1"/>
+    </ext>
+    <ext xmlns:x15="http://schemas.microsoft.com/office/spreadsheetml/2010/11/main" uri="{9260A510-F301-46a8-8635-F512D64BE5F5}">
+      <x15:timelineStyles defaultTimelineStyle="TimeSlicerStyleLight1"/>
+    </ext>
+  </extLst>
 </styleSheet>
 </file>
 
 <file path=xl/theme/theme1.xml><?xml version="1.0" encoding="utf-8"?>
-<a:theme xmlns:a="http://schemas.openxmlformats.org/drawingml/2006/main" name="Office Theme">
+<a:theme xmlns:a="http://schemas.openxmlformats.org/drawingml/2006/main" name="Tema do Office">
   <a:themeElements>
     <a:clrScheme name="Office">
       <a:dk1>
@@ -180,7 +163,7 @@
     </a:clrScheme>
     <a:fontScheme name="Office">
       <a:majorFont>
-        <a:latin typeface="Cambria"/>
+        <a:latin typeface="Cambria" panose="020F0302020204030204"/>
         <a:ea typeface=""/>
         <a:cs typeface=""/>
         <a:font script="Jpan" typeface="ＭＳ Ｐゴシック"/>
@@ -212,9 +195,10 @@
         <a:font script="Mong" typeface="Mongolian Baiti"/>
         <a:font script="Viet" typeface="Times New Roman"/>
         <a:font script="Uigh" typeface="Microsoft Uighur"/>
+        <a:font script="Geor" typeface="Sylfaen"/>
       </a:majorFont>
       <a:minorFont>
-        <a:latin typeface="Calibri"/>
+        <a:latin typeface="Calibri" panose="020F0502020204030204"/>
         <a:ea typeface=""/>
         <a:cs typeface=""/>
         <a:font script="Jpan" typeface="ＭＳ Ｐゴシック"/>
@@ -246,6 +230,7 @@
         <a:font script="Mong" typeface="Mongolian Baiti"/>
         <a:font script="Viet" typeface="Arial"/>
         <a:font script="Uigh" typeface="Microsoft Uighur"/>
+        <a:font script="Geor" typeface="Sylfaen"/>
       </a:minorFont>
     </a:fontScheme>
     <a:fmtScheme name="Office">
@@ -421,14 +406,16 @@
 </file>
 
 <file path=xl/worksheets/sheet1.xml><?xml version="1.0" encoding="utf-8"?>
-<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships">
-  <dimension ref="A1:G4"/>
+<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac">
+  <dimension ref="A1:G1"/>
   <sheetViews>
-    <sheetView tabSelected="1" workbookViewId="0"/>
+    <sheetView tabSelected="1" workbookViewId="0">
+      <selection activeCell="G11" sqref="G11"/>
+    </sheetView>
   </sheetViews>
-  <sheetFormatPr defaultRowHeight="15"/>
+  <sheetFormatPr defaultRowHeight="15" x14ac:dyDescent="0.25"/>
   <sheetData>
-    <row r="1" spans="1:7">
+    <row r="1" spans="1:7" x14ac:dyDescent="0.25">
       <c r="A1" s="1" t="s">
         <v>0</v>
       </c>
@@ -449,75 +436,6 @@
       </c>
       <c r="G1" s="1" t="s">
         <v>6</v>
-      </c>
-    </row>
-    <row r="2" spans="1:7">
-      <c r="A2" t="s">
-        <v>7</v>
-      </c>
-      <c r="B2" t="s">
-        <v>8</v>
-      </c>
-      <c r="C2" t="s">
-        <v>11</v>
-      </c>
-      <c r="D2" t="s">
-        <v>12</v>
-      </c>
-      <c r="E2" t="s">
-        <v>13</v>
-      </c>
-      <c r="F2" t="s">
-        <v>14</v>
-      </c>
-      <c r="G2" t="s">
-        <v>16</v>
-      </c>
-    </row>
-    <row r="3" spans="1:7">
-      <c r="A3" t="s">
-        <v>7</v>
-      </c>
-      <c r="B3" t="s">
-        <v>9</v>
-      </c>
-      <c r="C3" t="s">
-        <v>11</v>
-      </c>
-      <c r="D3" t="s">
-        <v>12</v>
-      </c>
-      <c r="E3" t="s">
-        <v>13</v>
-      </c>
-      <c r="F3" t="s">
-        <v>14</v>
-      </c>
-      <c r="G3" t="s">
-        <v>16</v>
-      </c>
-    </row>
-    <row r="4" spans="1:7">
-      <c r="A4" t="s">
-        <v>7</v>
-      </c>
-      <c r="B4" t="s">
-        <v>10</v>
-      </c>
-      <c r="C4" t="s">
-        <v>11</v>
-      </c>
-      <c r="D4" t="s">
-        <v>12</v>
-      </c>
-      <c r="E4" t="s">
-        <v>13</v>
-      </c>
-      <c r="F4" t="s">
-        <v>15</v>
-      </c>
-      <c r="G4" t="s">
-        <v>16</v>
       </c>
     </row>
   </sheetData>

</xml_diff>